<commit_message>
full end-to-end with diverse maps.
</commit_message>
<xml_diff>
--- a/web_gridworld/admin/schema.xlsx
+++ b/web_gridworld/admin/schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick\Documents\CODE\git\web_gridworld\web_gridworld\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D56E77-A986-4CAA-B586-1BB8C4AD9C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CEA09B-DAD9-451C-B341-1FE4ED8F53AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="1575" windowWidth="13170" windowHeight="11490" xr2:uid="{70362582-8895-4CB4-BE25-636310061903}"/>
+    <workbookView xWindow="2055" yWindow="2205" windowWidth="20625" windowHeight="11490" xr2:uid="{70362582-8895-4CB4-BE25-636310061903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>run_number</t>
-  </si>
-  <si>
-    <t>level_number</t>
-  </si>
-  <si>
     <t>run_timestamp</t>
   </si>
   <si>
@@ -87,10 +81,163 @@
     <t>username</t>
   </si>
   <si>
-    <t>user id</t>
-  </si>
-  <si>
     <t>the date-time stamp for this run</t>
+  </si>
+  <si>
+    <t>run_counter</t>
+  </si>
+  <si>
+    <t>first_color</t>
+  </si>
+  <si>
+    <t>second_color</t>
+  </si>
+  <si>
+    <t>third_color</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>competency</t>
+  </si>
+  <si>
+    <t>first_trust</t>
+  </si>
+  <si>
+    <t>second_trust</t>
+  </si>
+  <si>
+    <t>third_trust</t>
+  </si>
+  <si>
+    <t>open_question</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Robot color for first factor color (i.e. no conf. report)</t>
+  </si>
+  <si>
+    <t>Robot color for second factor color (i.e. conf. report)</t>
+  </si>
+  <si>
+    <t>Robot color for third factor color (i.e. seg. conf. report)</t>
+  </si>
+  <si>
+    <t>Accuracy of the statements [0,1]=[accurate, random]</t>
+  </si>
+  <si>
+    <t>Iinternal counter for runs</t>
+  </si>
+  <si>
+    <t>Integer ID of a user. Auto-incrementing</t>
+  </si>
+  <si>
+    <t>Performance of the robot [0,1]=[high performance, random performance]</t>
+  </si>
+  <si>
+    <t>Text username for this user</t>
+  </si>
+  <si>
+    <t>Trust rating for first factor</t>
+  </si>
+  <si>
+    <t>Trust rating for second factor</t>
+  </si>
+  <si>
+    <t>Trust rating for third factor</t>
+  </si>
+  <si>
+    <t>Open question/comments for this user at the end of the study</t>
+  </si>
+  <si>
+    <t>This user's password</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>integer (0,inf)</t>
+  </si>
+  <si>
+    <t>integer (0,max_runs)</t>
+  </si>
+  <si>
+    <t>integer (0,1,2)</t>
+  </si>
+  <si>
+    <t>integer (0,..,5)</t>
+  </si>
+  <si>
+    <t>Integer ID for this run. Auto-incrementing</t>
+  </si>
+  <si>
+    <t>Integer ID for this user.</t>
+  </si>
+  <si>
+    <t>The map ID for this run.</t>
+  </si>
+  <si>
+    <t>map_number</t>
+  </si>
+  <si>
+    <t>accuracy_level</t>
+  </si>
+  <si>
+    <t>competency_level</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>report_level</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>Confidence report statement for this run.</t>
+  </si>
+  <si>
+    <t>Level of this report (no report, conf report, segmented report)</t>
+  </si>
+  <si>
+    <t>The number of steps the human took</t>
+  </si>
+  <si>
+    <t>The number of steps the robot took</t>
+  </si>
+  <si>
+    <t>The outcome of this run (GOAL, DEAD)</t>
+  </si>
+  <si>
+    <t>The total time from start to goal in seconds</t>
+  </si>
+  <si>
+    <t>The total steps from start to goal</t>
+  </si>
+  <si>
+    <t>The total number of interventions</t>
+  </si>
+  <si>
+    <t>The total number of human steps across all interventions</t>
+  </si>
+  <si>
+    <t>The locations of each intervention (intervention start + stop)</t>
+  </si>
+  <si>
+    <t>list[integer]</t>
   </si>
 </sst>
 </file>
@@ -136,9 +283,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,115 +603,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8D8021-6DAB-4EF2-A2EC-469047FD0AB7}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>13</v>
+      <c r="C33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>